<commit_message>
modified the CSVFileFields to include Email
</commit_message>
<xml_diff>
--- a/CSVtoJSON_Application/Data/CSV/input.xlsx
+++ b/CSVtoJSON_Application/Data/CSV/input.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -919,7 +919,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="25.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="46" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
+    <col min="7" max="7" width="46.140625" customWidth="1"/>
+    <col min="8" max="8" width="41.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">

</xml_diff>